<commit_message>
created co2 WTP and updated SMR assumptions
</commit_message>
<xml_diff>
--- a/data/ship costs.xlsx
+++ b/data/ship costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s203679_dtu_dk/Documents/Dokumenter/DTU_Man/h2_system_dynamics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="194" documentId="8_{4DFCB4CD-F768-44D9-AD59-78ACB35E15C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9563494-A344-42D8-AD5E-E4BD7790B926}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="8_{4DFCB4CD-F768-44D9-AD59-78ACB35E15C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9479DE31-968A-476E-BAD6-0109979AF05C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{32D726C3-814A-45DA-8775-02AD4238E9C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{32D726C3-814A-45DA-8775-02AD4238E9C3}"/>
   </bookViews>
   <sheets>
     <sheet name="WTT" sheetId="1" r:id="rId1"/>
@@ -5807,7 +5807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C46E8A-A1F7-47EC-B088-0CEDC8A75426}">
   <dimension ref="A1:X39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>

</xml_diff>